<commit_message>
update weighted file with pulp and fix constraints
</commit_message>
<xml_diff>
--- a/Volunteer_Schedule.xlsx
+++ b/Volunteer_Schedule.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Schedule" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Schedule" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -481,12 +481,12 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Sarah Lee</t>
+          <t>John Doe</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>sarah.lee@example.com</t>
+          <t>john.doe@example.com</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -531,12 +531,12 @@
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>Emily White</t>
+          <t>Michael Brown</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>emily.white@example.com</t>
+          <t>michael.brown@example.com</t>
         </is>
       </c>
     </row>
@@ -553,12 +553,12 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Laura Black</t>
+          <t>Sarah Lee</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>laura.black@example.com</t>
+          <t>sarah.lee@example.com</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -583,12 +583,12 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>Sarah Lee</t>
+          <t>John Doe</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>sarah.lee@example.com</t>
+          <t>john.doe@example.com</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
@@ -645,12 +645,12 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>Emily White</t>
+          <t>Sarah Lee</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>emily.white@example.com</t>
+          <t>sarah.lee@example.com</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
@@ -667,12 +667,12 @@
     <row r="5">
       <c r="E5" t="inlineStr">
         <is>
-          <t>Michael Brown</t>
+          <t>Laura Black</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>michael.brown@example.com</t>
+          <t>laura.black@example.com</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
@@ -710,13 +710,13 @@
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="K1:L1"/>
     <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="M1:N1"/>
     <mergeCell ref="I1:J1"/>
-    <mergeCell ref="K1:L1"/>
-    <mergeCell ref="M1:N1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
fix contraints and obj
</commit_message>
<xml_diff>
--- a/Volunteer_Schedule.xlsx
+++ b/Volunteer_Schedule.xlsx
@@ -423,7 +423,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N5"/>
+  <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -471,42 +471,42 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>Nicole Thapa</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>nicole@uwaterloo.ca</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Harpreet Ghotra</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>harp@uwaterloo.ca</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Taylor Liu</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>twliew@uwaterloo.ca</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
           <t>Taylor Liew</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="H2" t="inlineStr">
         <is>
           <t>twliew@uwaterloo.ca</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Harpreet Ghotra</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>harp@uwaterloo.ca</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>Taylor Liu</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>twliew@uwaterloo.ca</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>Harpreet Ghotra</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>harp@uwaterloo.ca</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
@@ -543,62 +543,72 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Nicole Thapa</t>
+          <t>Bob Smith</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
+          <t>twliew@uwaterloo.ca</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Mary Popping</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>harp@uwaterloo.ca</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Kate Percy-Robb</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>kate@uwaterloo.ca</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Harpreet Ghotra</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>harp@uwaterloo.ca</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Dharsaa Bhagudeva</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>dhar@uwaterloo.ca</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>Patrick Star</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
           <t>nicole@uwaterloo.ca</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="M3" t="inlineStr">
         <is>
           <t>Mary Popping</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="N3" t="inlineStr">
         <is>
           <t>harp@uwaterloo.ca</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Kate Percy-Robb</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>kate@uwaterloo.ca</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>Al John</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>twliew@uwaterloo.ca</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>Dharsaa Bhagudeva</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>dhar@uwaterloo.ca</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>Kate Percy-Robb</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>kate@uwaterloo.ca</t>
         </is>
       </c>
     </row>
@@ -615,7 +625,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Bob Smith</t>
+          <t>Al John</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -625,12 +635,12 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Mary Popping</t>
+          <t>Dharsaa Bhagudeva</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>harp@uwaterloo.ca</t>
+          <t>dhar@uwaterloo.ca</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
@@ -645,12 +655,12 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>Patrick Star</t>
+          <t>Robin Hood</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>nicole@uwaterloo.ca</t>
+          <t>dhar@uwaterloo.ca</t>
         </is>
       </c>
     </row>
@@ -667,10 +677,32 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
+          <t>Mary Popping</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>harp@uwaterloo.ca</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
           <t>Robin Hood</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr">
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>dhar@uwaterloo.ca</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Robin Hood</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
         <is>
           <t>dhar@uwaterloo.ca</t>
         </is>

</xml_diff>